<commit_message>
Se agregaron los dos agentes de la quesera
</commit_message>
<xml_diff>
--- a/SCSimulator/DB Simulator.xlsx
+++ b/SCSimulator/DB Simulator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad Nacional\SEPRO\3.Programa\Plataformas\AnyLogic\Cadena de Suministro Industria Panificadora Palmira\SCBIP\SCBIP11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCSimulator\SCSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="236" yWindow="144" windowWidth="18956" windowHeight="8627" tabRatio="719" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="18960" windowHeight="8625" tabRatio="719" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Producto Terminado" sheetId="21" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="100">
   <si>
     <t>Levadura</t>
   </si>
@@ -997,13 +997,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="23"/>
@@ -1053,7 +1053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="D4" s="2"/>
@@ -1100,7 +1100,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
       <c r="D5" s="2"/>
@@ -1112,48 +1112,48 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
     </row>
@@ -1168,28 +1168,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="0.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="1" customWidth="1"/>
-    <col min="17" max="19" width="16.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20" customWidth="1"/>
-    <col min="21" max="21" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="0.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="1" customWidth="1"/>
+    <col min="18" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -1208,15 +1208,16 @@
       <c r="M1" s="40"/>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
-      <c r="Q1" s="26" t="s">
+      <c r="P1" s="40"/>
+      <c r="R1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="27"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
@@ -1245,15 +1246,16 @@
       </c>
       <c r="N2" s="40"/>
       <c r="O2" s="40"/>
-      <c r="Q2" s="26" t="s">
+      <c r="P2" s="40"/>
+      <c r="R2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="27"/>
       <c r="S2" s="27"/>
       <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
-    </row>
-    <row r="3" spans="1:21" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U2" s="27"/>
+      <c r="V2" s="28"/>
+    </row>
+    <row r="3" spans="1:22" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1291,28 +1293,31 @@
         <v>50</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1350,24 +1355,31 @@
         <v>0.1</v>
       </c>
       <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
         <v>0.2</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>80</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="S4" s="2">
+        <v>10</v>
+      </c>
       <c r="T4" s="2">
+        <v>10</v>
+      </c>
+      <c r="U4" s="2">
         <v>1.5</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>-76.2845778465271</v>
       </c>
@@ -1392,14 +1404,15 @@
       <c r="M5" s="2">
         <v>0.5</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
         <v>0.2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H6" s="1">
         <v>1</v>
       </c>
@@ -1418,14 +1431,15 @@
       <c r="M6" s="2">
         <v>0.1</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
         <v>0.8</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H7" s="1">
         <v>2</v>
       </c>
@@ -1444,14 +1458,15 @@
       <c r="M7" s="2">
         <v>0.3</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
         <v>0.2</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H8" s="1">
         <v>5</v>
       </c>
@@ -1470,24 +1485,25 @@
       <c r="M8" s="2">
         <v>0.1</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
         <v>0.5</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="R1:V1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1496,28 +1512,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="0.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="1" customWidth="1"/>
-    <col min="17" max="19" width="16.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20" customWidth="1"/>
-    <col min="21" max="21" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="0.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="1" customWidth="1"/>
+    <col min="18" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -1536,15 +1552,16 @@
       <c r="M1" s="40"/>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
-      <c r="Q1" s="26" t="s">
+      <c r="P1" s="40"/>
+      <c r="R1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="27"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1573,15 +1590,16 @@
       </c>
       <c r="N2" s="40"/>
       <c r="O2" s="40"/>
-      <c r="Q2" s="26" t="s">
+      <c r="P2" s="40"/>
+      <c r="R2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="27"/>
       <c r="S2" s="27"/>
       <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
-    </row>
-    <row r="3" spans="1:21" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U2" s="27"/>
+      <c r="V2" s="28"/>
+    </row>
+    <row r="3" spans="1:22" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1619,28 +1637,31 @@
         <v>50</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1678,24 +1699,31 @@
         <v>0.1</v>
       </c>
       <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
         <v>0.2</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>80</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="S4" s="2">
+        <v>10</v>
+      </c>
       <c r="T4" s="2">
+        <v>10</v>
+      </c>
+      <c r="U4" s="2">
         <v>1.5</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H5" s="2">
         <v>4</v>
       </c>
@@ -1714,14 +1742,15 @@
       <c r="M5" s="2">
         <v>0.5</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
         <v>0.2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H6" s="1">
         <v>1</v>
       </c>
@@ -1740,14 +1769,15 @@
       <c r="M6" s="2">
         <v>0.1</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
         <v>0.8</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H7" s="1">
         <v>2</v>
       </c>
@@ -1766,14 +1796,15 @@
       <c r="M7" s="2">
         <v>0.3</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
         <v>0.2</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H8" s="1">
         <v>5</v>
       </c>
@@ -1792,24 +1823,25 @@
       <c r="M8" s="2">
         <v>0.1</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
         <v>0.5</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="R1:V1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1824,22 +1856,22 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="8" max="9" width="0.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="9" width="0.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
     <col min="23" max="23" width="1" customWidth="1"/>
-    <col min="24" max="24" width="16.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1"/>
     <col min="25" max="25" width="20" customWidth="1"/>
-    <col min="26" max="26" width="21.88671875" customWidth="1"/>
+    <col min="26" max="26" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -1858,7 +1890,7 @@
       <c r="N1" s="45"/>
       <c r="O1" s="45"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1885,7 +1917,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="32"/>
     </row>
-    <row r="3" spans="1:15" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1926,7 +1958,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>98</v>
       </c>
@@ -1963,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J5" s="2">
         <v>2</v>
       </c>
@@ -1981,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J6" s="1">
         <v>3</v>
       </c>
@@ -1999,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J7" s="1">
         <v>4</v>
       </c>
@@ -2017,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J8" s="1">
         <v>5</v>
       </c>
@@ -2035,17 +2067,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>74</v>
       </c>
@@ -2072,14 +2104,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2093,7 +2125,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -2107,7 +2139,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2119,7 +2151,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2131,7 +2163,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2143,7 +2175,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2153,44 +2185,44 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
     </row>
@@ -2211,16 +2243,16 @@
       <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2246,7 +2278,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2269,7 +2301,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2287,7 +2319,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2305,7 +2337,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2323,7 +2355,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2341,7 +2373,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2350,7 +2382,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2359,42 +2391,42 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2415,32 +2447,32 @@
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -2482,7 +2514,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -2546,7 +2578,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -2645,7 +2677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2744,7 +2776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -2774,7 +2806,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -2828,32 +2860,32 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -2895,7 +2927,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -2959,7 +2991,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3058,7 +3090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -3157,7 +3189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -3187,7 +3219,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -3241,32 +3273,32 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -3308,7 +3340,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -3372,7 +3404,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3471,7 +3503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -3570,7 +3602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -3600,7 +3632,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -3654,32 +3686,32 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -3721,7 +3753,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -3785,7 +3817,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3884,7 +3916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -3983,7 +4015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4013,7 +4045,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4064,35 +4096,35 @@
   <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -4134,7 +4166,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -4198,7 +4230,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -4297,7 +4329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -4396,7 +4428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4426,7 +4458,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4476,36 +4508,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.109375" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="0.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.109375" customWidth="1"/>
-    <col min="32" max="32" width="23.33203125" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="32" max="32" width="23.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -4547,7 +4579,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
@@ -4611,7 +4643,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -4710,7 +4742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -4809,7 +4841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4839,7 +4871,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4863,22 +4895,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="V1:AC1"/>
     <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="S2:T2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="V2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrego el objeto vehiculo se configuro el objeto ruta
</commit_message>
<xml_diff>
--- a/SCSimulator/DB Simulator.xlsx
+++ b/SCSimulator/DB Simulator.xlsx
@@ -5,32 +5,33 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCSimulator\SCSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad Nacional\SEPRO\3.Programa\SCSimulator\SCSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="18960" windowHeight="8625" tabRatio="719" firstSheet="1" activeTab="10"/>
+    <workbookView minimized="1" xWindow="236" yWindow="144" windowWidth="18956" windowHeight="8627" tabRatio="719" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Producto Terminado" sheetId="21" r:id="rId1"/>
     <sheet name="Politicas de Gestion" sheetId="20" r:id="rId2"/>
     <sheet name="Materias Primas" sheetId="13" r:id="rId3"/>
-    <sheet name="Panaderia (5)" sheetId="36" r:id="rId4"/>
-    <sheet name="Panaderia (4)" sheetId="35" r:id="rId5"/>
-    <sheet name="Panaderia (3)" sheetId="34" r:id="rId6"/>
-    <sheet name="Panaderia (2)" sheetId="33" r:id="rId7"/>
-    <sheet name="Panaderia (1)" sheetId="32" r:id="rId8"/>
-    <sheet name="Panaderia (0)" sheetId="11" r:id="rId9"/>
-    <sheet name="Quesera (1)" sheetId="27" r:id="rId10"/>
-    <sheet name="Quesera (0)" sheetId="24" r:id="rId11"/>
-    <sheet name="Productor (0)" sheetId="25" r:id="rId12"/>
+    <sheet name="Vehiculos" sheetId="38" r:id="rId4"/>
+    <sheet name="Panaderia (5)" sheetId="36" r:id="rId5"/>
+    <sheet name="Panaderia (4)" sheetId="35" r:id="rId6"/>
+    <sheet name="Panaderia (3)" sheetId="34" r:id="rId7"/>
+    <sheet name="Panaderia (2)" sheetId="33" r:id="rId8"/>
+    <sheet name="Panaderia (1)" sheetId="32" r:id="rId9"/>
+    <sheet name="Panaderia (0)" sheetId="11" r:id="rId10"/>
+    <sheet name="Quesera (1)" sheetId="27" r:id="rId11"/>
+    <sheet name="Quesera (0)" sheetId="24" r:id="rId12"/>
+    <sheet name="Productor (0)" sheetId="25" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="108">
   <si>
     <t>Levadura</t>
   </si>
@@ -341,6 +342,31 @@
   </si>
   <si>
     <t>Politicas de Produccion - Producto Terminado</t>
+  </si>
+  <si>
+    <t>Bicicleta</t>
+  </si>
+  <si>
+    <t>Moto</t>
+  </si>
+  <si>
+    <t>Tipos de Transportes</t>
+  </si>
+  <si>
+    <t>Camion</t>
+  </si>
+  <si>
+    <t>Mensaje</t>
+  </si>
+  <si>
+    <t>Velocidad Media(km/h)</t>
+  </si>
+  <si>
+    <t>Capacidad     
+ (U.Pan)</t>
+  </si>
+  <si>
+    <t>Paquete</t>
   </si>
 </sst>
 </file>
@@ -543,7 +569,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,6 +709,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -994,16 +1023,16 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1057,7 @@
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="23"/>
@@ -1053,7 +1082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1088,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="D4" s="2"/>
@@ -1100,7 +1129,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
       <c r="D5" s="2"/>
@@ -1112,48 +1141,48 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
     </row>
@@ -1168,28 +1197,441 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI6"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
+    <col min="34" max="34" width="20" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="M1" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="32"/>
+      <c r="V1" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="32"/>
+      <c r="AE1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="40"/>
+      <c r="O2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="42"/>
+      <c r="V2" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="44"/>
+      <c r="X2" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AE2" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="28"/>
+    </row>
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="4"/>
+      <c r="V3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="21">
+        <v>-76.294727325439396</v>
+      </c>
+      <c r="C4" s="21">
+        <v>3.5375794937630101</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>500</v>
+      </c>
+      <c r="G4" s="2">
+        <v>300</v>
+      </c>
+      <c r="H4" s="2">
+        <v>50</v>
+      </c>
+      <c r="I4" s="2">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3</v>
+      </c>
+      <c r="O4" s="2">
+        <v>100</v>
+      </c>
+      <c r="P4" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>10</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2">
+        <v>3</v>
+      </c>
+      <c r="X4" s="2">
+        <v>100</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>18</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="M5" s="2">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3</v>
+      </c>
+      <c r="O5" s="2">
+        <v>100</v>
+      </c>
+      <c r="P5" s="1">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>20</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="M6" s="2">
+        <v>3</v>
+      </c>
+      <c r="N6" s="2">
+        <v>3</v>
+      </c>
+      <c r="O6" s="1">
+        <v>100</v>
+      </c>
+      <c r="P6" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>40</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="M1:T1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="0.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="0.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
     <col min="17" max="17" width="1" customWidth="1"/>
-    <col min="18" max="20" width="16.7109375" customWidth="1"/>
+    <col min="18" max="20" width="16.6640625" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" customWidth="1"/>
+    <col min="22" max="22" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -1217,7 +1659,7 @@
       <c r="U1" s="27"/>
       <c r="V1" s="28"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
@@ -1255,7 +1697,7 @@
       <c r="U2" s="27"/>
       <c r="V2" s="28"/>
     </row>
-    <row r="3" spans="1:22" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1317,7 +1759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1379,7 +1821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>-76.2845778465271</v>
       </c>
@@ -1412,7 +1854,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H6" s="1">
         <v>1</v>
       </c>
@@ -1439,7 +1881,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H7" s="1">
         <v>2</v>
       </c>
@@ -1466,345 +1908,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H8" s="1">
-        <v>5</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
-      <c r="J8" s="1">
-        <v>50</v>
-      </c>
-      <c r="K8" s="1">
-        <v>320</v>
-      </c>
-      <c r="L8" s="1">
-        <v>18</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:P1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="R2:V2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="0.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="17" max="17" width="1" customWidth="1"/>
-    <col min="18" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="H1" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="R1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="R2" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="28"/>
-    </row>
-    <row r="3" spans="1:22" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-76.285285949707003</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3.53183977750041</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-      <c r="J4" s="1">
-        <v>10</v>
-      </c>
-      <c r="K4" s="1">
-        <v>80</v>
-      </c>
-      <c r="L4" s="1">
-        <v>5</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R4" s="2">
-        <v>80</v>
-      </c>
-      <c r="S4" s="2">
-        <v>10</v>
-      </c>
-      <c r="T4" s="2">
-        <v>10</v>
-      </c>
-      <c r="U4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="V4" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1">
-        <v>90</v>
-      </c>
-      <c r="L5" s="1">
-        <v>10</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3</v>
-      </c>
-      <c r="J6" s="1">
-        <v>30</v>
-      </c>
-      <c r="K6" s="1">
-        <v>150</v>
-      </c>
-      <c r="L6" s="1">
-        <v>15</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="P6" s="2">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1">
-        <v>40</v>
-      </c>
-      <c r="K7" s="1">
-        <v>260</v>
-      </c>
-      <c r="L7" s="1">
-        <v>20</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H8" s="1">
         <v>5</v>
       </c>
@@ -1850,28 +1954,366 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="0.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="17" max="17" width="1" customWidth="1"/>
+    <col min="18" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="H1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="R1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="R2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="28"/>
+    </row>
+    <row r="3" spans="1:22" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-76.285285949707003</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.53183977750041</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1">
+        <v>80</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="2">
+        <v>80</v>
+      </c>
+      <c r="S4" s="2">
+        <v>10</v>
+      </c>
+      <c r="T4" s="2">
+        <v>10</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="V4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1">
+        <v>90</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1">
+        <v>150</v>
+      </c>
+      <c r="L6" s="1">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40</v>
+      </c>
+      <c r="K7" s="1">
+        <v>260</v>
+      </c>
+      <c r="L7" s="1">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>50</v>
+      </c>
+      <c r="K8" s="1">
+        <v>320</v>
+      </c>
+      <c r="L8" s="1">
+        <v>18</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:V2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="9" width="0.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="9" width="0.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
     <col min="23" max="23" width="1" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1"/>
     <col min="25" max="25" width="20" customWidth="1"/>
-    <col min="26" max="26" width="21.85546875" customWidth="1"/>
+    <col min="26" max="26" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -1890,7 +2332,7 @@
       <c r="N1" s="45"/>
       <c r="O1" s="45"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1917,7 +2359,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="32"/>
     </row>
-    <row r="3" spans="1:15" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1958,7 +2400,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>98</v>
       </c>
@@ -1995,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J5" s="2">
         <v>2</v>
       </c>
@@ -2013,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J6" s="1">
         <v>3</v>
       </c>
@@ -2031,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J7" s="1">
         <v>4</v>
       </c>
@@ -2049,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J8" s="1">
         <v>5</v>
       </c>
@@ -2067,17 +2509,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
       <c r="O17" t="s">
         <v>74</v>
       </c>
@@ -2104,14 +2546,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2125,7 +2567,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -2139,7 +2581,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2151,7 +2593,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2163,7 +2605,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2175,7 +2617,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2185,44 +2627,44 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
     </row>
@@ -2243,16 +2685,16 @@
       <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2720,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2301,7 +2743,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2319,7 +2761,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2337,7 +2779,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2355,7 +2797,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2373,7 +2815,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2382,7 +2824,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2391,42 +2833,42 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2441,38 +2883,148 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2">
+        <v>200</v>
+      </c>
+      <c r="D4" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -2514,7 +3066,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -2578,7 +3130,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -2677,7 +3229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2776,7 +3328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -2806,420 +3358,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M6" s="2">
-        <v>3</v>
-      </c>
-      <c r="N6" s="2">
-        <v>3</v>
-      </c>
-      <c r="O6" s="1">
-        <v>100</v>
-      </c>
-      <c r="P6" s="1">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>40</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:T1"/>
-    <mergeCell ref="V1:AC1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AE2:AF2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI6"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
-    <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="M1" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="32"/>
-      <c r="V1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="32"/>
-      <c r="AE1" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="T2" s="42"/>
-      <c r="V2" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="44"/>
-      <c r="X2" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AE2" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="28"/>
-    </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="21">
-        <v>-76.286058425903306</v>
-      </c>
-      <c r="C4" s="21">
-        <v>3.5223306172612698</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2">
-        <v>500</v>
-      </c>
-      <c r="G4" s="2">
-        <v>300</v>
-      </c>
-      <c r="H4" s="2">
-        <v>50</v>
-      </c>
-      <c r="I4" s="2">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>3</v>
-      </c>
-      <c r="O4" s="2">
-        <v>100</v>
-      </c>
-      <c r="P4" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>10</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="2">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="2">
-        <v>3</v>
-      </c>
-      <c r="X4" s="2">
-        <v>100</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>18</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>30</v>
-      </c>
-      <c r="AH4" s="2">
-        <v>60</v>
-      </c>
-      <c r="AI4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M5" s="2">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2">
-        <v>3</v>
-      </c>
-      <c r="O5" s="2">
-        <v>100</v>
-      </c>
-      <c r="P5" s="1">
-        <v>80</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>20</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -3273,32 +3412,32 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -3340,7 +3479,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -3404,7 +3543,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3503,15 +3642,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" s="21">
-        <v>-76.302838325500403</v>
+        <v>-76.286058425903306</v>
       </c>
       <c r="C4" s="21">
-        <v>3.52582160405374</v>
+        <v>3.5223306172612698</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -3526,13 +3665,13 @@
         <v>300</v>
       </c>
       <c r="H4" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -3602,7 +3741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -3632,7 +3771,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -3686,32 +3825,32 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -3753,7 +3892,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -3817,7 +3956,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -3916,15 +4055,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" s="21">
-        <v>-76.299684047698904</v>
+        <v>-76.302838325500403</v>
       </c>
       <c r="C4" s="21">
-        <v>3.5227589599039302</v>
+        <v>3.52582160405374</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -3939,10 +4078,10 @@
         <v>300</v>
       </c>
       <c r="H4" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2">
         <v>3</v>
@@ -4015,7 +4154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4045,7 +4184,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4096,35 +4235,35 @@
   <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -4166,7 +4305,7 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -4230,7 +4369,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -4329,15 +4468,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="20">
-        <v>-76.302945613860999</v>
+        <v>97</v>
+      </c>
+      <c r="B4" s="21">
+        <v>-76.299684047698904</v>
       </c>
       <c r="C4" s="21">
-        <v>3.53267503692551</v>
+        <v>3.5227589599039302</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -4352,13 +4491,13 @@
         <v>300</v>
       </c>
       <c r="H4" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I4" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -4428,7 +4567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4458,7 +4597,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4509,35 +4648,35 @@
   <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="1.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="0.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.109375" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="0.44140625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
@@ -4579,8 +4718,8 @@
       <c r="AH1" s="33"/>
       <c r="AI1" s="33"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="34" t="s">
@@ -4612,7 +4751,7 @@
       </c>
       <c r="P2" s="31"/>
       <c r="Q2" s="32"/>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="19" t="s">
         <v>49</v>
       </c>
       <c r="S2" s="41" t="s">
@@ -4643,7 +4782,7 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="28"/>
     </row>
-    <row r="3" spans="1:35" ht="60.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -4742,15 +4881,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="21">
-        <v>-76.294727325439396</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="20">
+        <v>-76.302945613860999</v>
       </c>
       <c r="C4" s="21">
-        <v>3.5375794937630101</v>
+        <v>3.53267503692551</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -4765,10 +4904,10 @@
         <v>300</v>
       </c>
       <c r="H4" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J4" s="2">
         <v>5</v>
@@ -4841,7 +4980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5" s="2">
         <v>2</v>
       </c>
@@ -4871,7 +5010,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M6" s="2">
         <v>3</v>
       </c>
@@ -4895,22 +5034,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="M1:T1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AE1:AI1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="M1:T1"/>
-    <mergeCell ref="S2:T2"/>
     <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="V2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>